<commit_message>
updating the pipeline naming convention
</commit_message>
<xml_diff>
--- a/docs/datasource_mappings.xlsx
+++ b/docs/datasource_mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmoud Shash\OneDrive - Tartu Ülikool\Töölaud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D49236-C5F6-4FA1-A145-50BF05A92038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78249FC-DCED-44B6-A3D0-4C0A13C024AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B2DDA58F-A7D7-4BB7-B84D-1618DB1E8A33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>Pipeline field</t>
   </si>
@@ -249,6 +249,135 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>sem_paper_ID</t>
+  </si>
+  <si>
+    <t>sem_s_STUDY</t>
+  </si>
+  <si>
+    <t>sem_url</t>
+  </si>
+  <si>
+    <t>sem_title</t>
+  </si>
+  <si>
+    <t>sem_venue</t>
+  </si>
+  <si>
+    <t>sem_year</t>
+  </si>
+  <si>
+    <t>sem_references[]</t>
+  </si>
+  <si>
+    <t>sem_publication_venue_name</t>
+  </si>
+  <si>
+    <t>sem_publication_venue_url</t>
+  </si>
+  <si>
+    <t>sem_publication_venue_id</t>
+  </si>
+  <si>
+    <t>sem_external_ids_doi</t>
+  </si>
+  <si>
+    <t>sem_publication_venue_type</t>
+  </si>
+  <si>
+    <t>sem_publication_venue_alternate_names</t>
+  </si>
+  <si>
+    <t>authors_name</t>
+  </si>
+  <si>
+    <t>authors_sequence</t>
+  </si>
+  <si>
+    <t>sem_authors_url</t>
+  </si>
+  <si>
+    <t>sem_authors_homepage</t>
+  </si>
+  <si>
+    <t>sem_authors_paperCount</t>
+  </si>
+  <si>
+    <t>sem_authors_citationCount</t>
+  </si>
+  <si>
+    <t>sem_authors_hIndex</t>
+  </si>
+  <si>
+    <t>sem_authors_aliases</t>
+  </si>
+  <si>
+    <t>sem_authors_affiliations</t>
+  </si>
+  <si>
+    <t>reference_count</t>
+  </si>
+  <si>
+    <t>citation_count</t>
+  </si>
+  <si>
+    <t>sem_influential_citation_count</t>
+  </si>
+  <si>
+    <t>sem_is_openaccess</t>
+  </si>
+  <si>
+    <t>sem_openaccess_location</t>
+  </si>
+  <si>
+    <t>General_category</t>
+  </si>
+  <si>
+    <t>publication_Date</t>
+  </si>
+  <si>
+    <t>sem_journal_name</t>
+  </si>
+  <si>
+    <t>sem_journal_volume</t>
+  </si>
+  <si>
+    <t>sem_external_arxi_id</t>
+  </si>
+  <si>
+    <t>license_start_date_time</t>
+  </si>
+  <si>
+    <t>license_start_content_version</t>
+  </si>
+  <si>
+    <t>license_start_delay_days</t>
+  </si>
+  <si>
+    <t>sem_citations[]</t>
+  </si>
+  <si>
+    <t>cross_lang</t>
+  </si>
+  <si>
+    <t>cross_score</t>
+  </si>
+  <si>
+    <t>cross_subject</t>
+  </si>
+  <si>
+    <t>cross_paper_url</t>
+  </si>
+  <si>
+    <t>cross_issn_type</t>
+  </si>
+  <si>
+    <t>cross_issn_number</t>
+  </si>
+  <si>
+    <t>cross_url</t>
   </si>
 </sst>
 </file>
@@ -625,12 +754,12 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
     <col min="2" max="2" width="40" style="3" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" customWidth="1"/>
     <col min="4" max="4" width="53.7109375" customWidth="1"/>
@@ -655,11 +784,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
       </c>
@@ -668,6 +803,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
@@ -676,6 +814,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
@@ -684,30 +825,45 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
@@ -716,6 +872,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
@@ -724,6 +883,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
@@ -732,6 +894,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>64</v>
       </c>
@@ -741,21 +906,33 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
@@ -763,22 +940,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -786,7 +975,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
       </c>
@@ -794,7 +986,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
@@ -802,22 +997,34 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
       <c r="B27" s="4" t="s">
         <v>29</v>
       </c>
@@ -828,7 +1035,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
@@ -836,7 +1046,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
       <c r="C29" s="2" t="s">
         <v>32</v>
       </c>
@@ -844,7 +1057,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
       <c r="B30" s="4" t="s">
         <v>34</v>
       </c>
@@ -855,27 +1071,42 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>106</v>
+      </c>
       <c r="C33" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
       <c r="C34" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
       <c r="C35" s="2" t="s">
         <v>44</v>
       </c>
@@ -883,7 +1114,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
       <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
@@ -891,17 +1125,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
       <c r="D37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
       <c r="D38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
@@ -909,17 +1152,26 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
       <c r="D40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>108</v>
+      </c>
       <c r="D41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
       <c r="B42" s="3" t="s">
         <v>60</v>
       </c>
@@ -927,22 +1179,34 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
       <c r="D43" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>109</v>
+      </c>
       <c r="D44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
       <c r="D45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
       <c r="D46" t="s">
         <v>63</v>
       </c>

</xml_diff>